<commit_message>
Updated use case 3
</commit_message>
<xml_diff>
--- a/myQfcProject/mycommon/src/main/resources/Book1.xlsx_error.xlsx
+++ b/myQfcProject/mycommon/src/main/resources/Book1.xlsx_error.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Error Data</t>
   </si>
@@ -83,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -123,23 +123,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>